<commit_message>
xlsw data files type=50 = updated the columns names for simplification
</commit_message>
<xml_diff>
--- a/data/data_to_use/time50engySpk.xlsx
+++ b/data/data_to_use/time50engySpk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benoît\Desktop\stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cdesbois/pg/chrisPg/centriG/data/data_to_use/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40983D26-650B-4E55-9E21-8F9BB2E399BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97591A51-4DFE-8D4E-A023-0078BBD47D3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,54 +90,6 @@
     <t>1649C_CXG4</t>
   </si>
   <si>
-    <t>spkfrndIsoStcDlat50Indisig</t>
-  </si>
-  <si>
-    <t>spkscpIsoStcDlat50</t>
-  </si>
-  <si>
-    <t>spkscpIsoStcDlat50Indisig</t>
-  </si>
-  <si>
-    <t>spkfcpIsoStcDlat50</t>
-  </si>
-  <si>
-    <t>spkfcpIsoStcDlat50Indisig</t>
-  </si>
-  <si>
-    <t>spkscfIsoStcDlat50</t>
-  </si>
-  <si>
-    <t>spkscfIsoStcDlat50Indisig</t>
-  </si>
-  <si>
-    <t>spkfcfIsoStcDlat50</t>
-  </si>
-  <si>
-    <t>spkfcfIsoStcDlat50Indisig</t>
-  </si>
-  <si>
-    <t>spkscpCrossStcDlat50</t>
-  </si>
-  <si>
-    <t>spkscpCrossStcDlat50Indisig</t>
-  </si>
-  <si>
-    <t>spkfcpCrossStcDlat50</t>
-  </si>
-  <si>
-    <t>spkfcpCrossStcDlat50Indisig</t>
-  </si>
-  <si>
-    <t>spksrndIsoStcDlat50</t>
-  </si>
-  <si>
-    <t>spksrndIsoStcDlat50Indisig</t>
-  </si>
-  <si>
-    <t>spkfrndIsoStcDlat50</t>
-  </si>
-  <si>
     <t>1641A_CXG5</t>
   </si>
   <si>
@@ -462,54 +414,6 @@
     <t>6.50000000000000E+0000</t>
   </si>
   <si>
-    <t>spkscpIsoStcDenergy</t>
-  </si>
-  <si>
-    <t>spkscpIsoStcDenergyIndisig</t>
-  </si>
-  <si>
-    <t>spkfcpIsoStcDenergy</t>
-  </si>
-  <si>
-    <t>spkfcpIsoStcDenergyIndisig</t>
-  </si>
-  <si>
-    <t>spkscfIsoStcDenergy</t>
-  </si>
-  <si>
-    <t>spkscfIsoStcDenergyIndisig</t>
-  </si>
-  <si>
-    <t>spkfcfIsoStcDenergy</t>
-  </si>
-  <si>
-    <t>spkfcfIsoStcDenergyIndisig</t>
-  </si>
-  <si>
-    <t>spkscpCrossStcDenergy</t>
-  </si>
-  <si>
-    <t>spkscpCrossStcDenergyIndisig</t>
-  </si>
-  <si>
-    <t>spkfcpCrossStcDenergy</t>
-  </si>
-  <si>
-    <t>spkfcpCrossStcDenergyIndisig</t>
-  </si>
-  <si>
-    <t>spksrndIsoStcDenergy</t>
-  </si>
-  <si>
-    <t>spksrndIsoStcDenergyIndisig</t>
-  </si>
-  <si>
-    <t>spkfrndIsoStcDenergy</t>
-  </si>
-  <si>
-    <t>spkfrndIsoStcDenergyIndisig</t>
-  </si>
-  <si>
     <t>6.07831001281738E-0001</t>
   </si>
   <si>
@@ -1036,13 +940,109 @@
   </si>
   <si>
     <t>8.66709113121033E-0001</t>
+  </si>
+  <si>
+    <t>spkscpIsoStcEngy</t>
+  </si>
+  <si>
+    <t>spkscpIsoStcEngySig</t>
+  </si>
+  <si>
+    <t>spkfcpIsoStcEngy</t>
+  </si>
+  <si>
+    <t>spkfcpIsoStcEngySig</t>
+  </si>
+  <si>
+    <t>spkscfIsoStcEngy</t>
+  </si>
+  <si>
+    <t>spkscfIsoStcEngySig</t>
+  </si>
+  <si>
+    <t>spkfcfIsoStcEngy</t>
+  </si>
+  <si>
+    <t>spkfcfIsoStcEngySig</t>
+  </si>
+  <si>
+    <t>spkscpCrossStcEngy</t>
+  </si>
+  <si>
+    <t>spkscpCrossStcEngySig</t>
+  </si>
+  <si>
+    <t>spkfcpCrossStcEngy</t>
+  </si>
+  <si>
+    <t>spkfcpCrossStcEngySig</t>
+  </si>
+  <si>
+    <t>spksrndIsoStcEngy</t>
+  </si>
+  <si>
+    <t>spksrndIsoStcEngySig</t>
+  </si>
+  <si>
+    <t>spkfrndIsoStcEngy</t>
+  </si>
+  <si>
+    <t>spkfrndIsoStcEngySig</t>
+  </si>
+  <si>
+    <t>spkscpIsoStcLat50</t>
+  </si>
+  <si>
+    <t>spkscpIsoStcLat50Sig</t>
+  </si>
+  <si>
+    <t>spkfcpIsoStcLat50</t>
+  </si>
+  <si>
+    <t>spkfcpIsoStcLat50Sig</t>
+  </si>
+  <si>
+    <t>spkscfIsoStcLat50</t>
+  </si>
+  <si>
+    <t>spkscfIsoStcLat50Sig</t>
+  </si>
+  <si>
+    <t>spkfcfIsoStcLat50</t>
+  </si>
+  <si>
+    <t>spkfcfIsoStcLat50Sig</t>
+  </si>
+  <si>
+    <t>spkscpCrossStcLat50</t>
+  </si>
+  <si>
+    <t>spkscpCrossStcLat50Sig</t>
+  </si>
+  <si>
+    <t>spkfcpCrossStcLat50</t>
+  </si>
+  <si>
+    <t>spkfcpCrossStcLat50Sig</t>
+  </si>
+  <si>
+    <t>spksrndIsoStcLat50</t>
+  </si>
+  <si>
+    <t>spksrndIsoStcLat50Sig</t>
+  </si>
+  <si>
+    <t>spkfrndIsoStcLat50</t>
+  </si>
+  <si>
+    <t>spkfrndIsoStcLat50Sig</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1091,7 +1091,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1394,2345 +1394,2345 @@
       <selection pane="topRight" activeCell="AG24" sqref="AG24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
-    <col min="5" max="9" width="27.42578125" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="9" width="27.5" customWidth="1"/>
+    <col min="10" max="10" width="23.1640625" customWidth="1"/>
     <col min="11" max="11" width="28" customWidth="1"/>
     <col min="12" max="12" width="25" customWidth="1"/>
-    <col min="13" max="17" width="29.28515625" customWidth="1"/>
-    <col min="18" max="18" width="26.42578125" customWidth="1"/>
+    <col min="13" max="17" width="29.33203125" customWidth="1"/>
+    <col min="18" max="18" width="26.5" customWidth="1"/>
     <col min="19" max="25" width="29" customWidth="1"/>
     <col min="26" max="26" width="23" customWidth="1"/>
-    <col min="27" max="27" width="32.85546875" customWidth="1"/>
-    <col min="28" max="28" width="26.140625" customWidth="1"/>
-    <col min="29" max="33" width="29.42578125" customWidth="1"/>
-    <col min="34" max="34" width="27.85546875" customWidth="1"/>
-    <col min="35" max="35" width="31.140625" customWidth="1"/>
+    <col min="27" max="27" width="32.83203125" customWidth="1"/>
+    <col min="28" max="28" width="26.1640625" customWidth="1"/>
+    <col min="29" max="33" width="29.5" customWidth="1"/>
+    <col min="34" max="34" width="27.83203125" customWidth="1"/>
+    <col min="35" max="35" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>321</v>
       </c>
       <c r="C1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E1" t="s">
+        <v>306</v>
+      </c>
+      <c r="F1" t="s">
+        <v>323</v>
+      </c>
+      <c r="G1" t="s">
+        <v>324</v>
+      </c>
+      <c r="H1" t="s">
+        <v>307</v>
+      </c>
+      <c r="I1" t="s">
+        <v>308</v>
+      </c>
+      <c r="J1" t="s">
+        <v>325</v>
+      </c>
+      <c r="K1" t="s">
+        <v>326</v>
+      </c>
+      <c r="L1" t="s">
+        <v>309</v>
+      </c>
+      <c r="M1" t="s">
+        <v>310</v>
+      </c>
+      <c r="N1" t="s">
+        <v>327</v>
+      </c>
+      <c r="O1" t="s">
+        <v>328</v>
+      </c>
+      <c r="P1" t="s">
+        <v>311</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>312</v>
+      </c>
+      <c r="R1" t="s">
+        <v>329</v>
+      </c>
+      <c r="S1" t="s">
+        <v>330</v>
+      </c>
+      <c r="T1" t="s">
+        <v>313</v>
+      </c>
+      <c r="U1" t="s">
+        <v>314</v>
+      </c>
+      <c r="V1" t="s">
+        <v>331</v>
+      </c>
+      <c r="W1" t="s">
+        <v>332</v>
+      </c>
+      <c r="X1" t="s">
+        <v>315</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>316</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>333</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>334</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>317</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>318</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>335</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>336</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>319</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I1" t="s">
-        <v>148</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>173</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
         <v>26</v>
       </c>
-      <c r="K1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" t="s">
-        <v>149</v>
-      </c>
-      <c r="M1" t="s">
-        <v>150</v>
-      </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>152</v>
-      </c>
-      <c r="R1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S1" t="s">
-        <v>31</v>
-      </c>
-      <c r="T1" t="s">
-        <v>153</v>
-      </c>
-      <c r="U1" t="s">
-        <v>154</v>
-      </c>
-      <c r="V1" t="s">
-        <v>32</v>
-      </c>
-      <c r="W1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X1" t="s">
-        <v>155</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>156</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>157</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>158</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>159</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>160</v>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>217</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>98</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2" t="s">
+        <v>239</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>283</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>183</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>205</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
-        <v>86</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2" t="s">
-        <v>227</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2" t="s">
-        <v>249</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2" t="s">
-        <v>114</v>
-      </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
-      <c r="X2" t="s">
-        <v>271</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AA2">
-        <v>1</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>293</v>
-      </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>315</v>
-      </c>
-      <c r="AG2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>162</v>
+        <v>130</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>184</v>
+        <v>152</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>206</v>
+        <v>174</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="S3">
         <v>0</v>
       </c>
       <c r="T3" t="s">
-        <v>250</v>
+        <v>218</v>
       </c>
       <c r="U3">
         <v>0</v>
       </c>
       <c r="V3" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="W3">
         <v>0</v>
       </c>
       <c r="X3" t="s">
-        <v>272</v>
+        <v>240</v>
       </c>
       <c r="Y3">
         <v>0</v>
       </c>
       <c r="Z3" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="AA3">
         <v>0</v>
       </c>
       <c r="AB3" t="s">
-        <v>294</v>
+        <v>262</v>
       </c>
       <c r="AC3">
         <v>0</v>
       </c>
       <c r="AD3" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="AE3">
         <v>0</v>
       </c>
       <c r="AF3" t="s">
-        <v>316</v>
+        <v>284</v>
       </c>
       <c r="AG3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>185</v>
+        <v>153</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>175</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
         <v>76</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4" t="s">
-        <v>207</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" t="s">
-        <v>92</v>
-      </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
       <c r="T4" t="s">
-        <v>251</v>
+        <v>219</v>
       </c>
       <c r="U4">
         <v>0</v>
       </c>
       <c r="V4" t="s">
+        <v>99</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4" t="s">
+        <v>241</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="s">
         <v>115</v>
       </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4" t="s">
-        <v>273</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>91</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>295</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>131</v>
-      </c>
       <c r="AE4">
         <v>0</v>
       </c>
       <c r="AF4" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
       <c r="AG4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>164</v>
+        <v>132</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="S5">
         <v>0</v>
       </c>
       <c r="T5" t="s">
-        <v>252</v>
+        <v>220</v>
       </c>
       <c r="U5">
         <v>0</v>
       </c>
       <c r="V5" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="W5">
         <v>0</v>
       </c>
       <c r="X5" t="s">
-        <v>274</v>
+        <v>242</v>
       </c>
       <c r="Y5">
         <v>0</v>
       </c>
       <c r="Z5" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="AA5">
         <v>0</v>
       </c>
       <c r="AB5" t="s">
-        <v>296</v>
+        <v>264</v>
       </c>
       <c r="AC5">
         <v>0</v>
       </c>
       <c r="AD5" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="AE5">
         <v>0</v>
       </c>
       <c r="AF5" t="s">
-        <v>318</v>
+        <v>286</v>
       </c>
       <c r="AG5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>187</v>
+        <v>155</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="Q6">
         <v>0</v>
       </c>
       <c r="R6" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="S6">
         <v>0</v>
       </c>
       <c r="T6" t="s">
-        <v>253</v>
+        <v>221</v>
       </c>
       <c r="U6">
         <v>0</v>
       </c>
       <c r="V6" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="W6">
         <v>0</v>
       </c>
       <c r="X6" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="Y6">
         <v>0</v>
       </c>
       <c r="Z6" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="AA6">
         <v>0</v>
       </c>
       <c r="AB6" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="AC6">
         <v>0</v>
       </c>
       <c r="AD6" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="AE6">
         <v>0</v>
       </c>
       <c r="AF6" t="s">
-        <v>319</v>
+        <v>287</v>
       </c>
       <c r="AG6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>188</v>
+        <v>156</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
+        <v>178</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
         <v>78</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" t="s">
-        <v>210</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7" t="s">
-        <v>94</v>
-      </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="S7">
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>254</v>
+        <v>222</v>
       </c>
       <c r="U7">
         <v>0</v>
       </c>
       <c r="V7" t="s">
+        <v>92</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="s">
         <v>108</v>
       </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7" t="s">
-        <v>276</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>124</v>
-      </c>
       <c r="AA7">
         <v>0</v>
       </c>
       <c r="AB7" t="s">
-        <v>298</v>
+        <v>266</v>
       </c>
       <c r="AC7">
         <v>0</v>
       </c>
       <c r="AD7" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="AE7">
         <v>0</v>
       </c>
       <c r="AF7" t="s">
-        <v>320</v>
+        <v>288</v>
       </c>
       <c r="AG7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>189</v>
+        <v>157</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>179</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8" t="s">
         <v>79</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8" t="s">
-        <v>211</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8" t="s">
-        <v>95</v>
-      </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="S8">
         <v>0</v>
       </c>
       <c r="T8" t="s">
-        <v>255</v>
+        <v>223</v>
       </c>
       <c r="U8">
         <v>0</v>
       </c>
       <c r="V8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="W8">
         <v>0</v>
       </c>
       <c r="X8" t="s">
-        <v>277</v>
+        <v>245</v>
       </c>
       <c r="Y8">
         <v>0</v>
       </c>
       <c r="Z8" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="AA8">
         <v>0</v>
       </c>
       <c r="AB8" t="s">
-        <v>299</v>
+        <v>267</v>
       </c>
       <c r="AC8">
         <v>0</v>
       </c>
       <c r="AD8" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="AE8">
         <v>0</v>
       </c>
       <c r="AF8" t="s">
-        <v>321</v>
+        <v>289</v>
       </c>
       <c r="AG8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>190</v>
+        <v>158</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
       <c r="M9">
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="Q9">
         <v>0</v>
       </c>
       <c r="R9" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="S9">
         <v>1</v>
       </c>
       <c r="T9" t="s">
-        <v>256</v>
+        <v>224</v>
       </c>
       <c r="U9">
         <v>0</v>
       </c>
       <c r="V9" t="s">
+        <v>102</v>
+      </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9" t="s">
+        <v>246</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>268</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9" t="s">
         <v>118</v>
       </c>
-      <c r="W9">
-        <v>1</v>
-      </c>
-      <c r="X9" t="s">
-        <v>278</v>
-      </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>125</v>
-      </c>
-      <c r="AA9">
-        <v>0</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>300</v>
-      </c>
-      <c r="AC9">
-        <v>0</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>134</v>
-      </c>
       <c r="AE9">
         <v>0</v>
       </c>
       <c r="AF9" t="s">
-        <v>322</v>
+        <v>290</v>
       </c>
       <c r="AG9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>213</v>
+        <v>181</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="S10">
         <v>0</v>
       </c>
       <c r="T10" t="s">
-        <v>257</v>
+        <v>225</v>
       </c>
       <c r="U10">
         <v>0</v>
       </c>
       <c r="V10" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="W10">
         <v>1</v>
       </c>
       <c r="X10" t="s">
-        <v>279</v>
+        <v>247</v>
       </c>
       <c r="Y10">
         <v>0</v>
       </c>
       <c r="Z10" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="AA10">
         <v>0</v>
       </c>
       <c r="AB10" t="s">
-        <v>301</v>
+        <v>269</v>
       </c>
       <c r="AC10">
         <v>0</v>
       </c>
       <c r="AD10" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="AE10">
         <v>1</v>
       </c>
       <c r="AF10" t="s">
-        <v>323</v>
+        <v>291</v>
       </c>
       <c r="AG10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>192</v>
+        <v>160</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="Q11">
         <v>0</v>
       </c>
       <c r="R11" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="S11">
         <v>0</v>
       </c>
       <c r="T11" t="s">
-        <v>258</v>
+        <v>226</v>
       </c>
       <c r="U11">
         <v>0</v>
       </c>
       <c r="V11" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="W11">
         <v>0</v>
       </c>
       <c r="X11" t="s">
-        <v>280</v>
+        <v>248</v>
       </c>
       <c r="Y11">
         <v>0</v>
       </c>
       <c r="Z11" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="AA11">
         <v>0</v>
       </c>
       <c r="AB11" t="s">
-        <v>302</v>
+        <v>270</v>
       </c>
       <c r="AC11">
         <v>0</v>
       </c>
       <c r="AD11" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="AE11">
         <v>0</v>
       </c>
       <c r="AF11" t="s">
-        <v>324</v>
+        <v>292</v>
       </c>
       <c r="AG11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>171</v>
+        <v>139</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="Q12">
         <v>1</v>
       </c>
       <c r="R12" t="s">
+        <v>66</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12" t="s">
+        <v>227</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12" t="s">
         <v>82</v>
       </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12" t="s">
-        <v>259</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12" t="s">
-        <v>98</v>
-      </c>
       <c r="W12">
         <v>0</v>
       </c>
       <c r="X12" t="s">
-        <v>281</v>
+        <v>249</v>
       </c>
       <c r="Y12">
         <v>0</v>
       </c>
       <c r="Z12" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="AA12">
         <v>0</v>
       </c>
       <c r="AB12" t="s">
-        <v>303</v>
+        <v>271</v>
       </c>
       <c r="AC12">
         <v>0</v>
       </c>
       <c r="AD12" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="AE12">
         <v>0</v>
       </c>
       <c r="AF12" t="s">
-        <v>325</v>
+        <v>293</v>
       </c>
       <c r="AG12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>194</v>
+        <v>162</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>238</v>
+        <v>206</v>
       </c>
       <c r="Q13">
         <v>0</v>
       </c>
       <c r="R13" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="S13">
         <v>0</v>
       </c>
       <c r="T13" t="s">
-        <v>260</v>
+        <v>228</v>
       </c>
       <c r="U13">
         <v>0</v>
       </c>
       <c r="V13" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="W13">
         <v>0</v>
       </c>
       <c r="X13" t="s">
-        <v>282</v>
+        <v>250</v>
       </c>
       <c r="Y13">
         <v>0</v>
       </c>
       <c r="Z13" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="AA13">
         <v>0</v>
       </c>
       <c r="AB13" t="s">
-        <v>304</v>
+        <v>272</v>
       </c>
       <c r="AC13">
         <v>0</v>
       </c>
       <c r="AD13" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="AE13">
         <v>0</v>
       </c>
       <c r="AF13" t="s">
-        <v>326</v>
+        <v>294</v>
       </c>
       <c r="AG13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>195</v>
+        <v>163</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>239</v>
+        <v>207</v>
       </c>
       <c r="Q14">
         <v>0</v>
       </c>
       <c r="R14" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="S14">
         <v>0</v>
       </c>
       <c r="T14" t="s">
-        <v>261</v>
+        <v>229</v>
       </c>
       <c r="U14">
         <v>0</v>
       </c>
       <c r="V14" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="W14">
         <v>0</v>
       </c>
       <c r="X14" t="s">
-        <v>283</v>
+        <v>251</v>
       </c>
       <c r="Y14">
         <v>0</v>
       </c>
       <c r="Z14" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="AA14">
         <v>0</v>
       </c>
       <c r="AB14" t="s">
-        <v>305</v>
+        <v>273</v>
       </c>
       <c r="AC14">
         <v>0</v>
       </c>
       <c r="AD14" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="AE14">
         <v>0</v>
       </c>
       <c r="AF14" t="s">
-        <v>327</v>
+        <v>295</v>
       </c>
       <c r="AG14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>174</v>
+        <v>142</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>196</v>
+        <v>164</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>240</v>
+        <v>208</v>
       </c>
       <c r="Q15">
         <v>0</v>
       </c>
       <c r="R15" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="S15">
         <v>0</v>
       </c>
       <c r="T15" t="s">
-        <v>262</v>
+        <v>230</v>
       </c>
       <c r="U15">
         <v>0</v>
       </c>
       <c r="V15" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="W15">
         <v>0</v>
       </c>
       <c r="X15" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
       <c r="Y15">
         <v>0</v>
       </c>
       <c r="Z15" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="AA15">
         <v>0</v>
       </c>
       <c r="AB15" t="s">
-        <v>306</v>
+        <v>274</v>
       </c>
       <c r="AC15">
         <v>0</v>
       </c>
       <c r="AD15" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="AE15">
         <v>0</v>
       </c>
       <c r="AF15" t="s">
-        <v>328</v>
+        <v>296</v>
       </c>
       <c r="AG15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>165</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
         <v>70</v>
       </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>197</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16" t="s">
-        <v>86</v>
-      </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>219</v>
+        <v>187</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16" t="s">
+        <v>43</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16" t="s">
+        <v>88</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16" t="s">
+        <v>231</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16" t="s">
         <v>59</v>
       </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16" t="s">
-        <v>104</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="T16" t="s">
-        <v>263</v>
-      </c>
-      <c r="U16">
-        <v>0</v>
-      </c>
-      <c r="V16" t="s">
-        <v>75</v>
-      </c>
       <c r="W16">
         <v>0</v>
       </c>
       <c r="X16" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="Y16">
         <v>0</v>
       </c>
       <c r="Z16" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="AA16">
         <v>0</v>
       </c>
       <c r="AB16" t="s">
-        <v>307</v>
+        <v>275</v>
       </c>
       <c r="AC16">
         <v>0</v>
       </c>
       <c r="AD16" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="AE16">
         <v>0</v>
       </c>
       <c r="AF16" t="s">
-        <v>329</v>
+        <v>297</v>
       </c>
       <c r="AG16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>198</v>
+        <v>166</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>242</v>
+        <v>210</v>
       </c>
       <c r="Q17">
         <v>0</v>
       </c>
       <c r="R17" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="S17">
         <v>0</v>
       </c>
       <c r="T17" t="s">
-        <v>264</v>
+        <v>232</v>
       </c>
       <c r="U17">
         <v>1</v>
       </c>
       <c r="V17" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="W17">
         <v>1</v>
       </c>
       <c r="X17" t="s">
-        <v>286</v>
+        <v>254</v>
       </c>
       <c r="Y17">
         <v>0</v>
       </c>
       <c r="Z17" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="AA17">
         <v>0</v>
       </c>
       <c r="AB17" t="s">
-        <v>308</v>
+        <v>276</v>
       </c>
       <c r="AC17">
         <v>1</v>
       </c>
       <c r="AD17" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="AE17">
         <v>1</v>
       </c>
       <c r="AF17" t="s">
-        <v>330</v>
+        <v>298</v>
       </c>
       <c r="AG17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
         <v>55</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18" t="s">
-        <v>177</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18" t="s">
-        <v>71</v>
-      </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>199</v>
+        <v>167</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="N18" t="s">
+        <v>39</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18" t="s">
+        <v>94</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18" t="s">
+        <v>233</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18" t="s">
         <v>55</v>
       </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18" t="s">
-        <v>110</v>
-      </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18" t="s">
-        <v>265</v>
-      </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
-      <c r="V18" t="s">
-        <v>71</v>
-      </c>
       <c r="W18">
         <v>0</v>
       </c>
       <c r="X18" t="s">
-        <v>287</v>
+        <v>255</v>
       </c>
       <c r="Y18">
         <v>1</v>
       </c>
       <c r="Z18" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="AA18">
         <v>0</v>
       </c>
       <c r="AB18" t="s">
-        <v>309</v>
+        <v>277</v>
       </c>
       <c r="AC18">
         <v>0</v>
       </c>
       <c r="AD18" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="AE18">
         <v>0</v>
       </c>
       <c r="AF18" t="s">
-        <v>331</v>
+        <v>299</v>
       </c>
       <c r="AG18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>146</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
         <v>56</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19" t="s">
-        <v>178</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>168</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>190</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19" t="s">
+        <v>28</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19" t="s">
+        <v>95</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19" t="s">
+        <v>234</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19" t="s">
+        <v>105</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19" t="s">
+        <v>256</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>278</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>300</v>
+      </c>
+      <c r="AG19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>169</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
         <v>72</v>
       </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19" t="s">
-        <v>200</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19" t="s">
-        <v>44</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19" t="s">
-        <v>222</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19" t="s">
-        <v>111</v>
-      </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
-      <c r="T19" t="s">
-        <v>266</v>
-      </c>
-      <c r="U19">
-        <v>0</v>
-      </c>
-      <c r="V19" t="s">
-        <v>121</v>
-      </c>
-      <c r="W19">
-        <v>0</v>
-      </c>
-      <c r="X19" t="s">
-        <v>288</v>
-      </c>
-      <c r="Y19">
-        <v>0</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>129</v>
-      </c>
-      <c r="AA19">
-        <v>0</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>310</v>
-      </c>
-      <c r="AC19">
-        <v>0</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>99</v>
-      </c>
-      <c r="AE19">
-        <v>0</v>
-      </c>
-      <c r="AF19" t="s">
-        <v>332</v>
-      </c>
-      <c r="AG19">
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>191</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20" t="s">
+        <v>84</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20" t="s">
+        <v>96</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20" t="s">
+        <v>235</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20" t="s">
+        <v>98</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>279</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>301</v>
+      </c>
+      <c r="AG20">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>179</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>201</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20" t="s">
-        <v>88</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20" t="s">
-        <v>223</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20" t="s">
-        <v>100</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20" t="s">
-        <v>245</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20" t="s">
-        <v>112</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20" t="s">
-        <v>267</v>
-      </c>
-      <c r="U20">
-        <v>0</v>
-      </c>
-      <c r="V20" t="s">
-        <v>114</v>
-      </c>
-      <c r="W20">
-        <v>0</v>
-      </c>
-      <c r="X20" t="s">
-        <v>289</v>
-      </c>
-      <c r="Y20">
-        <v>0</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA20">
-        <v>0</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>311</v>
-      </c>
-      <c r="AC20">
-        <v>0</v>
-      </c>
-      <c r="AD20" t="s">
-        <v>142</v>
-      </c>
-      <c r="AE20">
-        <v>0</v>
-      </c>
-      <c r="AF20" t="s">
-        <v>333</v>
-      </c>
-      <c r="AG20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
       <c r="I21">
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="K21">
         <v>1</v>
       </c>
       <c r="L21" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="O21">
         <v>0</v>
       </c>
       <c r="P21" t="s">
-        <v>246</v>
+        <v>214</v>
       </c>
       <c r="Q21">
         <v>0</v>
       </c>
       <c r="R21" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="S21">
         <v>1</v>
       </c>
       <c r="T21" t="s">
-        <v>268</v>
+        <v>236</v>
       </c>
       <c r="U21">
         <v>0</v>
       </c>
       <c r="V21" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="W21">
         <v>1</v>
       </c>
       <c r="X21" t="s">
-        <v>290</v>
+        <v>258</v>
       </c>
       <c r="Y21">
         <v>0</v>
       </c>
       <c r="Z21" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="AA21">
         <v>1</v>
       </c>
       <c r="AB21" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="AC21">
         <v>0</v>
       </c>
       <c r="AD21" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="AE21">
         <v>0</v>
       </c>
       <c r="AF21" t="s">
-        <v>334</v>
+        <v>302</v>
       </c>
       <c r="AG21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>171</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>73</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22" t="s">
+        <v>193</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22" t="s">
+        <v>85</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22" t="s">
+        <v>45</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22" t="s">
+        <v>237</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22" t="s">
+        <v>106</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22" t="s">
         <v>59</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22" t="s">
-        <v>181</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22" t="s">
-        <v>203</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22" t="s">
-        <v>89</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22" t="s">
-        <v>225</v>
-      </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
-      <c r="N22" t="s">
-        <v>101</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22" t="s">
-        <v>247</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22" t="s">
-        <v>61</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-      <c r="T22" t="s">
-        <v>269</v>
-      </c>
-      <c r="U22">
-        <v>0</v>
-      </c>
-      <c r="V22" t="s">
-        <v>122</v>
-      </c>
-      <c r="W22">
-        <v>1</v>
-      </c>
-      <c r="X22" t="s">
-        <v>291</v>
-      </c>
-      <c r="Y22">
-        <v>0</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>75</v>
-      </c>
       <c r="AA22">
         <v>0</v>
       </c>
       <c r="AB22" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="AC22">
         <v>1</v>
       </c>
       <c r="AD22" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="AE22">
         <v>1</v>
       </c>
       <c r="AF22" t="s">
-        <v>335</v>
+        <v>303</v>
       </c>
       <c r="AG22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>182</v>
+        <v>150</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>172</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23" t="s">
         <v>74</v>
       </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23" t="s">
-        <v>204</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23" t="s">
-        <v>90</v>
-      </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
       <c r="M23">
         <v>0</v>
       </c>
       <c r="N23" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="O23">
         <v>0</v>
       </c>
       <c r="P23" t="s">
-        <v>248</v>
+        <v>216</v>
       </c>
       <c r="Q23">
         <v>0</v>
       </c>
       <c r="R23" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="S23">
         <v>0</v>
       </c>
       <c r="T23" t="s">
-        <v>270</v>
+        <v>238</v>
       </c>
       <c r="U23">
         <v>0</v>
       </c>
       <c r="V23" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="W23">
         <v>0</v>
       </c>
       <c r="X23" t="s">
-        <v>292</v>
+        <v>260</v>
       </c>
       <c r="Y23">
         <v>0</v>
       </c>
       <c r="Z23" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="AA23">
         <v>0</v>
       </c>
       <c r="AB23" t="s">
-        <v>314</v>
+        <v>282</v>
       </c>
       <c r="AC23">
         <v>0</v>
       </c>
       <c r="AD23" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="AE23">
         <v>0</v>
       </c>
       <c r="AF23" t="s">
-        <v>336</v>
+        <v>304</v>
       </c>
       <c r="AG23">
         <v>0</v>

</xml_diff>

<commit_message>
stats corrected for one spiking cell time50engySpk.xlsx Benoît
</commit_message>
<xml_diff>
--- a/data/data_to_use/time50engySpk.xlsx
+++ b/data/data_to_use/time50engySpk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cdesbois/pg/chrisPg/centriG/data/data_to_use/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\travail\sourcecode\developing\paper\centriG\data\data_to_use\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97591A51-4DFE-8D4E-A023-0078BBD47D3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D66E14-6192-49D9-B33B-C20ACA2ECBA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20880" yWindow="1320" windowWidth="15870" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="339">
   <si>
     <t>Neuron</t>
   </si>
@@ -102,9 +102,6 @@
     <t>-1.00000001490116E-0001</t>
   </si>
   <si>
-    <t>2.26000003814697E+0001</t>
-  </si>
-  <si>
     <t>3.79999995231628E+0000</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>5.80000019073486E+0000</t>
   </si>
   <si>
-    <t>2.28999996185303E+0001</t>
-  </si>
-  <si>
     <t>-6.00000023841858E-0001</t>
   </si>
   <si>
@@ -207,9 +201,6 @@
     <t>3.40000009536743E+0000</t>
   </si>
   <si>
-    <t>-7.30000019073486E+0000</t>
-  </si>
-  <si>
     <t>1.70000004768372E+0000</t>
   </si>
   <si>
@@ -324,9 +315,6 @@
     <t>7.40000009536743E+0000</t>
   </si>
   <si>
-    <t>-5.09999990463257E+0000</t>
-  </si>
-  <si>
     <t>2.53999996185303E+0001</t>
   </si>
   <si>
@@ -372,9 +360,6 @@
     <t>1.16999998092651E+0001</t>
   </si>
   <si>
-    <t>-3.90000009536743E+0000</t>
-  </si>
-  <si>
     <t>1.29999995231628E+0000</t>
   </si>
   <si>
@@ -1036,16 +1021,43 @@
   </si>
   <si>
     <t>spkfrndIsoStcLat50Sig</t>
+  </si>
+  <si>
+    <t>2.30000000000000E+0001</t>
+  </si>
+  <si>
+    <t>1.82000007629395E+0001</t>
+  </si>
+  <si>
+    <t>-5.90000009536743E+0000</t>
+  </si>
+  <si>
+    <t>7.80000019073486E+0000</t>
+  </si>
+  <si>
+    <t>-1.11999998092651E+0001</t>
+  </si>
+  <si>
+    <t>-4.59999990463257E+0000</t>
+  </si>
+  <si>
+    <t>2.92999992370606E+0001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1071,8 +1083,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1091,7 +1104,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1390,133 +1403,133 @@
   <dimension ref="A1:AG23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AG24" sqref="AG24"/>
+      <pane xSplit="1" topLeftCell="AE1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" customWidth="1"/>
-    <col min="5" max="9" width="27.5" customWidth="1"/>
-    <col min="10" max="10" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+    <col min="5" max="9" width="27.42578125" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" customWidth="1"/>
     <col min="11" max="11" width="28" customWidth="1"/>
     <col min="12" max="12" width="25" customWidth="1"/>
-    <col min="13" max="17" width="29.33203125" customWidth="1"/>
-    <col min="18" max="18" width="26.5" customWidth="1"/>
+    <col min="13" max="17" width="29.28515625" customWidth="1"/>
+    <col min="18" max="18" width="26.42578125" customWidth="1"/>
     <col min="19" max="25" width="29" customWidth="1"/>
     <col min="26" max="26" width="23" customWidth="1"/>
-    <col min="27" max="27" width="32.83203125" customWidth="1"/>
-    <col min="28" max="28" width="26.1640625" customWidth="1"/>
-    <col min="29" max="33" width="29.5" customWidth="1"/>
-    <col min="34" max="34" width="27.83203125" customWidth="1"/>
-    <col min="35" max="35" width="31.1640625" customWidth="1"/>
+    <col min="27" max="27" width="32.85546875" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" customWidth="1"/>
+    <col min="29" max="33" width="29.42578125" customWidth="1"/>
+    <col min="34" max="34" width="27.85546875" customWidth="1"/>
+    <col min="35" max="35" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G1" t="s">
+        <v>319</v>
+      </c>
+      <c r="H1" t="s">
+        <v>302</v>
+      </c>
+      <c r="I1" t="s">
+        <v>303</v>
+      </c>
+      <c r="J1" t="s">
+        <v>320</v>
+      </c>
+      <c r="K1" t="s">
         <v>321</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" t="s">
+        <v>304</v>
+      </c>
+      <c r="M1" t="s">
+        <v>305</v>
+      </c>
+      <c r="N1" t="s">
         <v>322</v>
       </c>
-      <c r="D1" t="s">
-        <v>305</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="O1" t="s">
+        <v>323</v>
+      </c>
+      <c r="P1" t="s">
         <v>306</v>
       </c>
-      <c r="F1" t="s">
-        <v>323</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="Q1" t="s">
+        <v>307</v>
+      </c>
+      <c r="R1" t="s">
         <v>324</v>
       </c>
-      <c r="H1" t="s">
-        <v>307</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="S1" t="s">
+        <v>325</v>
+      </c>
+      <c r="T1" t="s">
         <v>308</v>
       </c>
-      <c r="J1" t="s">
-        <v>325</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="U1" t="s">
+        <v>309</v>
+      </c>
+      <c r="V1" t="s">
         <v>326</v>
       </c>
-      <c r="L1" t="s">
-        <v>309</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="W1" t="s">
+        <v>327</v>
+      </c>
+      <c r="X1" t="s">
         <v>310</v>
       </c>
-      <c r="N1" t="s">
-        <v>327</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="Y1" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z1" t="s">
         <v>328</v>
       </c>
-      <c r="P1" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="AA1" t="s">
+        <v>329</v>
+      </c>
+      <c r="AB1" t="s">
         <v>312</v>
       </c>
-      <c r="R1" t="s">
-        <v>329</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="AC1" t="s">
+        <v>313</v>
+      </c>
+      <c r="AD1" t="s">
         <v>330</v>
       </c>
-      <c r="T1" t="s">
-        <v>313</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="AE1" t="s">
+        <v>331</v>
+      </c>
+      <c r="AF1" t="s">
         <v>314</v>
       </c>
-      <c r="V1" t="s">
-        <v>331</v>
-      </c>
-      <c r="W1" t="s">
-        <v>332</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="AG1" t="s">
         <v>315</v>
       </c>
-      <c r="Y1" t="s">
-        <v>316</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>333</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>334</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>317</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>318</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>335</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>336</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>319</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>320</v>
-      </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1527,97 +1540,97 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S2">
         <v>0</v>
       </c>
       <c r="T2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="U2">
         <v>0</v>
       </c>
       <c r="V2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="W2">
         <v>1</v>
       </c>
       <c r="X2" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="Y2">
         <v>0</v>
       </c>
       <c r="Z2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="AA2">
         <v>1</v>
       </c>
       <c r="AB2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="AC2">
         <v>0</v>
       </c>
       <c r="AD2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="AE2">
         <v>0</v>
       </c>
       <c r="AF2" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="AG2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1628,483 +1641,483 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="S3">
         <v>0</v>
       </c>
       <c r="T3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="U3">
         <v>0</v>
       </c>
       <c r="V3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="W3">
         <v>0</v>
       </c>
       <c r="X3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="Y3">
         <v>0</v>
       </c>
       <c r="Z3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="AA3">
         <v>0</v>
       </c>
       <c r="AB3" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="AC3">
         <v>0</v>
       </c>
       <c r="AD3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AE3">
         <v>0</v>
       </c>
       <c r="AF3" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="AG3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
-      <c r="A4" t="s">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>25</v>
+      <c r="B4" s="1" t="s">
+        <v>332</v>
       </c>
       <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>131</v>
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>46</v>
+      <c r="F4" s="1" t="s">
+        <v>333</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" t="s">
-        <v>153</v>
+      <c r="H4" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
-      <c r="J4" t="s">
-        <v>60</v>
+      <c r="J4" s="1" t="s">
+        <v>334</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4" t="s">
-        <v>175</v>
+      <c r="L4" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
-      <c r="N4" t="s">
-        <v>76</v>
+      <c r="N4" s="1" t="s">
+        <v>335</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
-      <c r="P4" t="s">
-        <v>197</v>
+      <c r="P4" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
-      <c r="R4" t="s">
-        <v>60</v>
+      <c r="R4" s="1" t="s">
+        <v>336</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
-      <c r="T4" t="s">
-        <v>219</v>
+      <c r="T4" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="U4">
         <v>0</v>
       </c>
-      <c r="V4" t="s">
-        <v>99</v>
+      <c r="V4" s="1" t="s">
+        <v>337</v>
       </c>
       <c r="W4">
         <v>0</v>
       </c>
-      <c r="X4" t="s">
-        <v>241</v>
+      <c r="X4" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="Y4">
         <v>0</v>
       </c>
-      <c r="Z4" t="s">
-        <v>75</v>
+      <c r="Z4" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="AA4">
         <v>0</v>
       </c>
-      <c r="AB4" t="s">
-        <v>263</v>
+      <c r="AB4" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="AC4">
         <v>0</v>
       </c>
-      <c r="AD4" t="s">
-        <v>115</v>
+      <c r="AD4" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>285</v>
+        <v>1</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>280</v>
       </c>
       <c r="AG4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="S5">
         <v>0</v>
       </c>
       <c r="T5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="U5">
         <v>0</v>
       </c>
       <c r="V5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="W5">
         <v>0</v>
       </c>
       <c r="X5" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="Y5">
         <v>0</v>
       </c>
       <c r="Z5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AA5">
         <v>0</v>
       </c>
       <c r="AB5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="AC5">
         <v>0</v>
       </c>
       <c r="AD5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="AE5">
         <v>0</v>
       </c>
       <c r="AF5" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="AG5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="Q6">
         <v>0</v>
       </c>
       <c r="R6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="S6">
         <v>0</v>
       </c>
       <c r="T6" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="U6">
         <v>0</v>
       </c>
       <c r="V6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="W6">
         <v>0</v>
       </c>
       <c r="X6" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="Y6">
         <v>0</v>
       </c>
       <c r="Z6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AA6">
         <v>0</v>
       </c>
       <c r="AB6" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="AC6">
         <v>0</v>
       </c>
       <c r="AD6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="AE6">
         <v>0</v>
       </c>
       <c r="AF6" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="AG6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7" t="s">
+        <v>75</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7" t="s">
         <v>78</v>
       </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7" t="s">
-        <v>81</v>
-      </c>
       <c r="S7">
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="U7">
         <v>0</v>
       </c>
       <c r="V7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="W7">
         <v>0</v>
       </c>
       <c r="X7" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="Y7">
         <v>0</v>
       </c>
       <c r="Z7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="AA7">
         <v>0</v>
       </c>
       <c r="AB7" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="AC7">
         <v>0</v>
@@ -2116,84 +2129,84 @@
         <v>0</v>
       </c>
       <c r="AF7" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="AG7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="S8">
         <v>0</v>
       </c>
       <c r="T8" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="U8">
         <v>0</v>
       </c>
       <c r="V8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="W8">
         <v>0</v>
       </c>
       <c r="X8" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="Y8">
         <v>0</v>
@@ -2205,1207 +2218,1207 @@
         <v>0</v>
       </c>
       <c r="AB8" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="AC8">
         <v>0</v>
       </c>
       <c r="AD8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AE8">
         <v>0</v>
       </c>
       <c r="AF8" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="AG8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="M9">
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="Q9">
         <v>0</v>
       </c>
       <c r="R9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="S9">
         <v>1</v>
       </c>
       <c r="T9" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="U9">
         <v>0</v>
       </c>
       <c r="V9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="W9">
         <v>1</v>
       </c>
       <c r="X9" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="Y9">
         <v>0</v>
       </c>
       <c r="Z9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="AA9">
         <v>0</v>
       </c>
       <c r="AB9" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="AC9">
         <v>0</v>
       </c>
       <c r="AD9" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="AE9">
         <v>0</v>
       </c>
       <c r="AF9" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="AG9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="S10">
         <v>0</v>
       </c>
       <c r="T10" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="U10">
         <v>0</v>
       </c>
       <c r="V10" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="W10">
         <v>1</v>
       </c>
       <c r="X10" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="Y10">
         <v>0</v>
       </c>
       <c r="Z10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA10">
         <v>0</v>
       </c>
       <c r="AB10" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="AC10">
         <v>0</v>
       </c>
       <c r="AD10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="AE10">
         <v>1</v>
       </c>
       <c r="AF10" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="AG10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="Q11">
         <v>0</v>
       </c>
       <c r="R11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="S11">
         <v>0</v>
       </c>
       <c r="T11" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="U11">
         <v>0</v>
       </c>
       <c r="V11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="W11">
         <v>0</v>
       </c>
       <c r="X11" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="Y11">
         <v>0</v>
       </c>
       <c r="Z11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA11">
         <v>0</v>
       </c>
       <c r="AB11" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="AC11">
         <v>0</v>
       </c>
       <c r="AD11" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="AE11">
         <v>0</v>
       </c>
       <c r="AF11" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="AG11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="Q12">
         <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="S12">
         <v>0</v>
       </c>
       <c r="T12" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="U12">
         <v>0</v>
       </c>
       <c r="V12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="W12">
         <v>0</v>
       </c>
       <c r="X12" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="Y12">
         <v>0</v>
       </c>
       <c r="Z12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA12">
         <v>0</v>
       </c>
       <c r="AB12" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="AC12">
         <v>0</v>
       </c>
       <c r="AD12" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="AE12">
         <v>0</v>
       </c>
       <c r="AF12" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="AG12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>179</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" t="s">
         <v>68</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13" t="s">
-        <v>184</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13" t="s">
-        <v>71</v>
-      </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="Q13">
         <v>0</v>
       </c>
       <c r="R13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="S13">
         <v>0</v>
       </c>
       <c r="T13" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="U13">
         <v>0</v>
       </c>
       <c r="V13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="W13">
         <v>0</v>
       </c>
       <c r="X13" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="Y13">
         <v>0</v>
       </c>
       <c r="Z13" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="AA13">
         <v>0</v>
       </c>
       <c r="AB13" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="AC13">
         <v>0</v>
       </c>
       <c r="AD13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="AE13">
         <v>0</v>
       </c>
       <c r="AF13" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="AG13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="Q14">
         <v>0</v>
       </c>
       <c r="R14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="S14">
         <v>0</v>
       </c>
       <c r="T14" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="U14">
         <v>0</v>
       </c>
       <c r="V14" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="W14">
         <v>0</v>
       </c>
       <c r="X14" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="Y14">
         <v>0</v>
       </c>
       <c r="Z14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA14">
         <v>0</v>
       </c>
       <c r="AB14" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="AC14">
         <v>0</v>
       </c>
       <c r="AD14" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="AE14">
         <v>0</v>
       </c>
       <c r="AF14" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="AG14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="Q15">
         <v>0</v>
       </c>
       <c r="R15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="S15">
         <v>0</v>
       </c>
       <c r="T15" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="U15">
         <v>0</v>
       </c>
       <c r="V15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="W15">
         <v>0</v>
       </c>
       <c r="X15" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="Y15">
         <v>0</v>
       </c>
       <c r="Z15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AA15">
         <v>0</v>
       </c>
       <c r="AB15" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AC15">
         <v>0</v>
       </c>
       <c r="AD15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AE15">
         <v>0</v>
       </c>
       <c r="AF15" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="AG15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="Q16">
         <v>0</v>
       </c>
       <c r="R16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="S16">
         <v>0</v>
       </c>
       <c r="T16" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="U16">
         <v>0</v>
       </c>
       <c r="V16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="W16">
         <v>0</v>
       </c>
       <c r="X16" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="Y16">
         <v>0</v>
       </c>
       <c r="Z16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA16">
         <v>0</v>
       </c>
       <c r="AB16" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AC16">
         <v>0</v>
       </c>
       <c r="AD16" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="AE16">
         <v>0</v>
       </c>
       <c r="AF16" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="AG16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="Q17">
         <v>0</v>
       </c>
       <c r="R17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S17">
         <v>0</v>
       </c>
       <c r="T17" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="U17">
         <v>1</v>
       </c>
       <c r="V17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="W17">
         <v>1</v>
       </c>
       <c r="X17" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="Y17">
         <v>0</v>
       </c>
       <c r="Z17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AA17">
         <v>0</v>
       </c>
       <c r="AB17" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="AC17">
         <v>1</v>
       </c>
       <c r="AD17" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="AE17">
         <v>1</v>
       </c>
       <c r="AF17" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="AG17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:33">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O18">
         <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="Q18">
         <v>0</v>
       </c>
       <c r="R18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="S18">
         <v>0</v>
       </c>
       <c r="T18" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="U18">
         <v>0</v>
       </c>
       <c r="V18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W18">
         <v>0</v>
       </c>
       <c r="X18" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="Y18">
         <v>1</v>
       </c>
       <c r="Z18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="AA18">
         <v>0</v>
       </c>
       <c r="AB18" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="AC18">
         <v>0</v>
       </c>
       <c r="AD18" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="AE18">
         <v>0</v>
       </c>
       <c r="AF18" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="AG18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:33">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="M19">
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="Q19">
         <v>0</v>
       </c>
       <c r="R19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="S19">
         <v>0</v>
       </c>
       <c r="T19" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="U19">
         <v>0</v>
       </c>
       <c r="V19" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="W19">
         <v>0</v>
       </c>
       <c r="X19" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="Y19">
         <v>0</v>
       </c>
       <c r="Z19" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="AA19">
         <v>0</v>
       </c>
       <c r="AB19" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="AC19">
         <v>0</v>
       </c>
       <c r="AD19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AE19">
         <v>0</v>
       </c>
       <c r="AF19" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="AG19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:33">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O20">
         <v>0</v>
       </c>
       <c r="P20" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="Q20">
         <v>0</v>
       </c>
       <c r="R20" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="S20">
         <v>0</v>
       </c>
       <c r="T20" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="U20">
         <v>0</v>
       </c>
       <c r="V20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="W20">
         <v>0</v>
       </c>
       <c r="X20" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="Y20">
         <v>0</v>
@@ -3417,322 +3430,322 @@
         <v>0</v>
       </c>
       <c r="AB20" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="AC20">
         <v>0</v>
       </c>
       <c r="AD20" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="AE20">
         <v>0</v>
       </c>
       <c r="AF20" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="AG20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:33">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>143</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>165</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21" t="s">
+        <v>187</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21" t="s">
+        <v>78</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21" t="s">
         <v>42</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21" t="s">
-        <v>148</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21" t="s">
-        <v>170</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21" t="s">
-        <v>33</v>
-      </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
-      <c r="L21" t="s">
-        <v>192</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21" t="s">
-        <v>81</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21" t="s">
-        <v>214</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21" t="s">
-        <v>43</v>
-      </c>
       <c r="S21">
         <v>1</v>
       </c>
       <c r="T21" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="U21">
         <v>0</v>
       </c>
       <c r="V21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="W21">
         <v>1</v>
       </c>
       <c r="X21" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="Y21">
         <v>0</v>
       </c>
       <c r="Z21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="AA21">
         <v>1</v>
       </c>
       <c r="AB21" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="AC21">
         <v>0</v>
       </c>
       <c r="AD21" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="AE21">
         <v>0</v>
       </c>
       <c r="AF21" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="AG21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:33">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>166</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>70</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22" t="s">
+        <v>188</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22" t="s">
+        <v>82</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22" t="s">
+        <v>44</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22" t="s">
+        <v>232</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22" t="s">
+        <v>102</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22" t="s">
+        <v>254</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22" t="s">
         <v>57</v>
       </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22" t="s">
-        <v>171</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22" t="s">
-        <v>73</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22" t="s">
-        <v>193</v>
-      </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
-      <c r="N22" t="s">
-        <v>85</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22" t="s">
-        <v>45</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-      <c r="T22" t="s">
-        <v>237</v>
-      </c>
-      <c r="U22">
-        <v>0</v>
-      </c>
-      <c r="V22" t="s">
-        <v>106</v>
-      </c>
-      <c r="W22">
-        <v>1</v>
-      </c>
-      <c r="X22" t="s">
-        <v>259</v>
-      </c>
-      <c r="Y22">
-        <v>0</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>59</v>
-      </c>
       <c r="AA22">
         <v>0</v>
       </c>
       <c r="AB22" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="AC22">
         <v>1</v>
       </c>
       <c r="AD22" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="AE22">
         <v>1</v>
       </c>
       <c r="AF22" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="AG22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:33">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I23">
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="M23">
         <v>0</v>
       </c>
       <c r="N23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="O23">
         <v>0</v>
       </c>
       <c r="P23" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="Q23">
         <v>0</v>
       </c>
       <c r="R23" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="S23">
         <v>0</v>
       </c>
       <c r="T23" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="U23">
         <v>0</v>
       </c>
       <c r="V23" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="W23">
         <v>0</v>
       </c>
       <c r="X23" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="Y23">
         <v>0</v>
       </c>
       <c r="Z23" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="AA23">
         <v>0</v>
       </c>
       <c r="AB23" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="AC23">
         <v>0</v>
       </c>
       <c r="AD23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AE23">
         <v>0</v>
       </c>
       <c r="AF23" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="AG23">
         <v>0</v>
@@ -3740,5 +3753,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>